<commit_message>
Primera version para revision de indra
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-DigitoVerificador.xlsx
+++ b/docs/StructureDefinition-DigitoVerificador.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="102">
   <si>
     <t>Property</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-01-20T14:40:00-03:00</t>
+    <t>2023-01-25T12:03:32-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -317,10 +317,6 @@
   </si>
   <si>
     <t>Extension.value[x]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer
-</t>
   </si>
   <si>
     <t>Value of extension</t>
@@ -1237,13 +1233,13 @@
         <v>72</v>
       </c>
       <c r="K6" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="L6" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="L6" t="s" s="2">
+      <c r="M6" t="s" s="2">
         <v>100</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>101</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1306,7 +1302,7 @@
         <v>72</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AK6" t="s" s="2">
         <v>97</v>

</xml_diff>